<commit_message>
fix: update import paths and README for xlsx-parser; adjust parse-table-style defaults
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D335D-9A34-8B4C-B284-0B632627E2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF3A95A-9FFC-614B-B2EF-D4FEFE116EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
+    <workbookView xWindow="9720" yWindow="6700" windowWidth="29400" windowHeight="17460" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -689,7 +689,7 @@
     <row r="3" spans="1:4" ht="25" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>0</v>

</xml_diff>